<commit_message>
H1 Windows All updated
</commit_message>
<xml_diff>
--- a/ML/Windows_H1.xlsx
+++ b/ML/Windows_H1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7820" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="H1-1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="H1-4" sheetId="8" r:id="rId4"/>
     <sheet name="H1-5" sheetId="5" r:id="rId5"/>
     <sheet name="H1-6" sheetId="4" r:id="rId6"/>
+    <sheet name="Test" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'H1-1'!$A$1:$S$47</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="72">
   <si>
     <t>On Cluster</t>
   </si>
@@ -230,6 +231,27 @@
   <si>
     <t>'Dishwasher (Phase 2)'</t>
   </si>
+  <si>
+    <t>Test set</t>
+  </si>
+  <si>
+    <t>OnIdx</t>
+  </si>
+  <si>
+    <t>OffIdx</t>
+  </si>
+  <si>
+    <t>lenOn</t>
+  </si>
+  <si>
+    <t>lenOff</t>
+  </si>
+  <si>
+    <t>Dryer (phase2)'</t>
+  </si>
+  <si>
+    <t>Central Vacuum (phase1)'</t>
+  </si>
 </sst>
 </file>
 
@@ -302,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -447,6 +469,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,7 +777,7 @@
   <dimension ref="A1:AE47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1273,7 +1319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -5651,7 +5697,7 @@
   <dimension ref="A1:AE210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8374,7 +8420,7 @@
   <dimension ref="A1:AE210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9106,8 +9152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9865,4 +9911,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="58"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="52"/>
+      <c r="Z1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>16</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="B3" s="7">
+        <v>8</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="B4" s="35">
+        <v>11</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21">
+        <v>35</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tex update - minor
</commit_message>
<xml_diff>
--- a/ML/Windows_H1.xlsx
+++ b/ML/Windows_H1.xlsx
@@ -9918,7 +9918,7 @@
   <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10012,9 +10012,6 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
       <c r="B5" s="21">
         <v>35</v>
       </c>

</xml_diff>